<commit_message>
import espacios académicos funcionando
</commit_message>
<xml_diff>
--- a/public/storage/espacios.xlsx
+++ b/public/storage/espacios.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -247,12 +247,23 @@
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Si no tiene dejar vacio</t>
+          <t>Jose Daniel Isaza Hernandez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Si no tiene dejar vacio</t>
         </r>
       </text>
     </comment>
@@ -285,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
   <si>
     <t>codigo</t>
   </si>
@@ -1167,621 +1178,6 @@
 • Identificar los tipos de lectura que un profesional CIDBA debe asumir de acuerdo a la situación y contexto real.
 • Presentar una propuesta de animación a la lectura aplicada en un contexto concreto.</t>
   </si>
-  <si>
-    <t xml:space="preserve">La lectura es una herramienta fundamental para la formación del ser humano, ya que se convierte en un instrumento para generar placer, conocimiento, capacidad crítica, reflexiva y propositiva frente a las ideas plasmadas por el otro. La lectura no es un proceso innato en el ser humano, es un aprendizaje que requiere motivación, dedicación, esfuerzo y ante todo un guía que provea de las herramientas fundamentales para adquirir el hábito de la lectura, no sólo por placer, sino como una necesidad fundamental para entender el mundo, entender el pensamiento del otro e interactuar con el mundo cotidiano.
-El bibliotecario desde su Unidad de Información tiene la responsabilidad de incidir en los procesos socio-culturales de la población. Es por ello, que no sólo se requiere que sea un buen lector, sino que logre animar a otros por la lectura. Lo anterior puede lograrse, en tanto se conozcan diferentes estrategias para animar a leer a diferentes públicos.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Foros: Son momentos de encuentro en los que tendremos la oportunidad de conversar sobre algunos temas de interés general con respecto a la asignatura, o una reflexión acerca de nuestro propio acto lector y alguna exploración de conocimientos previos acerca de la lectura. También es una oportunidad para establecer un diálogo y conocimiento de los estudiantes y docentes entre sí.  
-• TALLERES: Realizar los talleres y actividades propuestos dentro del tiempo estipulado por el docente; para lo cual debe revisar continuamente la plataforma. 
-Lea cuidadosamente los temas y amplíelos según la bibliografía recomendada en cada unidad. Para la elaboración de los documentos, guárdelos como archivo en word, o en formato pdf. Todos los documentos deben tener las normas APA (versión 6).
-Presente los trabajos con una correcta redacción, puntuación y ortografía. Estos aspectos inciden en la nota de sus trabajos. Imagínese un animador lector con fallas en estos aspectos. Cuente siempre con nuestra disposición para acompañarlo en su proceso de aprendizaje. En caso de tener alguna dificultad académica o metodológica cumpla con el conducto regular establecido en el Estatuto Estudiantil.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como se puede observar en el cuadro del punto 8, tenemos 4 actividades evaluativas: 
-Talleres: en esta tarea se ve reflejada una metodología teórico-práctica, debido a que no sólo deben leer los materiales de la plataforma, sino indagar y aplicar los conocimientos en el desarrollo de la tarea.  
-Cuestionario en el que se presentan varias preguntas  sobre los contenidos vistos en la unidad correspondiente. 
-Trabajo final  también es teórico –práctico, los estudiantes deben tener mucha claridad conceptual adquirida a través de las lecturas de las diferentes unidades temáticas, aprender a planear una propuesta y ejecutarla.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• ¿Qué es lectura? Clases de lectura. Reflexión acerca del acto lector personal y el papel que juega en la formación como profesionales de CIDBA.
-• Establecer la diferencia entre Animación y Promoción Lectora, conociendo las estrategias y acciones propias de cada una.
-• Definición del texto y las clases de texto, sus características y propiedades. Reconocer las diferentes clases de textos.
-• Instrucciones para presentar una Propuesta de Animación Lectora.
-</t>
-  </si>
-  <si>
-    <t>Los estudiantes inicialmente conocerán algunos conceptos relacionados con la lectura y reflexionarán sobre su propio acto lector, teniendo en cuenta los contenidos de cada Unidad Didáctica. Además, tendrán la oportunidad de visitar algunas bibliotecas y espacios en los que se realizan programas de animación y promoción lectora y espacios para practicar acciones y estrategias de animación.</t>
-  </si>
-  <si>
-    <t>Tomando como premisa la responsabilidad social que se contempla en el Proyecto Educativo Institucional de la Universidad y del Programa de CIDBA, se propone una reflexión acerca de la misión y función del bibliotecólogo en el mundo de hoy, en cuanto a la formación de lectores y mejores ciudadanos, para el desarrollo cultural y social de las comunidades. Es así como se contemplan propuestas relacionadas con el acto lector y dirigidas a diferentes grupos humanos desde las diferentes unidades de información.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta asignatura ha sido la base para formular proyectos de Grado, cuyas temáticas han estado relacionadas con el Tema de la Animación Lectora. En la línea de investigación: Acto Lector, se prepara a los estudiantes para que visualicen desde la asignatura, posibles temas de investigación que son susceptibles de trabajar en el Semillero de Investigación. De igual manera, se sientan las bases para el aprendizaje relacionado con la formulación de proyectos en el campo de la Animación Lectora.  
-Mediante la realización de las distintas actividades teórico-prácticas se fomenta la investigación, el autoaprendizaje y la autorregulación del estudiante y el trabajo colaborativo como parte fundamental del aprendizaje virtual y la plataforma MOODLE.
-</t>
-  </si>
-  <si>
-    <t>Unidad 1 Historia de los archivos                              Unidad 2 Definición de Archivística                Unidad 3 Los archivos y sus fases de formación               Unidad 4 Los archivos sistemas y normas</t>
-  </si>
-  <si>
-    <t>Unidad 1. Lectura y clases de lectura                   Unidad 2. Animación vs promoción lectora                Unidad 3. Tipologías textuales          Unidad 4. Propuesta de animación lectora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La animación a la lectura. María Monserrat Sarto.
- Este texto busca dar estrategias de animación a la lectura, para personas que tienen vínculo con bibliotecas y la educación, a través del juego vincula al animador de una manera activa, permitiéndole ser el mediador entre el autor, el libro y el lector.
-* Cómo analizamos relatos infantiles y juveniles. Gemma Lluch. Grupo editorial Norma. 
-La autora presenta un modelo de análisis de la literatura infantil con otros tipos de literatura y de narraciones, teniendo como eje central las conceptualizaciones de la narrativa y sus elementos, pasando por la tradición oral, hasta llegar al vertiginoso mundo de la tecnología y su relación con la literatura.
-*Proceso al gramaticalismo: La aventura de leer y escribir. Pablo Zapata Lerga. 
-Este texto presenta de una manera didáctica la experiencia de los docentes frente a la animación de la lectura, una tarea difícil, pero no imposible. Plantea aspectos de la lectura y escritura, a partir del análisis de los lectores de acuerdo a sus edades, gustos y capacidades. El autor da recomendaciones de lo que se debe y no se debe hacer en el arduo, pero satisfactorio trabajo de la animación de la lectura.
-*Documentos empresariales: cómo elaborarlos. Héctor Pérez Grajales. En este texto se encuentra la funcionalidad, objetivo y estructura de los diferentes documentos que circulan en una empresa, aunque su enfoque está dirigido a la redacción es importante tenerlo en cuenta, ya que el conocimiento de dicha estructura como tipología textual, permite entender e interpretar el mensaje de los contenidos.
-*Los procesos de la lectura. Hacia la producción interactiva de los sentidos. Fabio Jurado Valencia y Guillermo Bustamante Zamudio. Ed. Magisterio.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• http://pitbox.wordpress.com/2011/07/26/el-texto-narrativo-estructura-y-elementosdel-texto-narrativo/
- • http://es.scribd.com/doc/6145826/Estructura-Del-Texto-Argumentativo1
- • http://salonhogar.net/Salones/Espanol/4-6/Texto_descriptivo.htm
- • http://aulalibre.es/spip.php?article20
- • http://www.um.es/gtiweb/jgomez/bibedu/pautasorg/intro/animlect.htm
- • http://catamorales.wordpress.com/prueba-1/
- • http://www.cedinpro.edu.co/contenido_c/publicaciones/formadores_vi_DAP.pdf 
-• http://www.complejoideal.com/module/sites/ideal/galerias/alcalaEduca/descargas/en cuentroProfesorado/TallerA/LECTURAEFICAZ.pdf
- • http://www.abc.com.py/edicion-impresa/suplementos/escolar/fabulas-en-ingles593348.html 
-</t>
-  </si>
-  <si>
-    <t>Julio 28 de 2017 – Actualización del syllabus a la plantilla requerida en el PAC- Esp. Amparo Betancourt Gómez - Docente.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esp. Patricia Villegas Celis- Coordinadora de Área Acto Lector.
-</t>
-  </si>
-  <si>
-    <t>ESTADÍSTICA DESCRIPTIVA</t>
-  </si>
-  <si>
-    <t>La misión de nuestro programa apunta hacia la formación integral de la persona y del profesional en la gestión y la administración de información, por medio de la estadística descriptiva contribuimos brindando herramientas suficientes para el adecuado manejo de la información.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividades
-Foro general: durante cada semana se crea un foro con diversos debates (Espacio para compartir bibliografía, espacio para formular inquietudes, seguimiento del aprendizaje) (Estará activo desde la fecha en que se abre hasta por dos semanas con fecha de corte, el siguiente sábado a las 11:50 p.m.)
-Trabajo Nº1 (Evalúa las unidades 1 y 2), contiene ejercicios de aplicación de los contenidos vistos, debe ser digitado con su respectivo proceso matemático y la interpretación de las respuestas.
-Trabajo Nº2 (Evalúa las unidades 3,4 y 5) contiene ejercicios de aplicación de los contenidos vistos, debe ser digitado con su respectivo proceso matemático y la interpretación de las respuestas.
-Trabajo Nº3 (Aplicación en contexto) Determinan una variable cuantitativa en su entorno laboral, le realizan seguimiento y posteriormente el análisis estadístico que involucra todos los contenidos vistos en el espacio académico. (Preámbulo al proceso de investigación)
-Evaluación (En plataforma) Consiste en un cuestionario de preguntas con selección múltiple con única respuesta, diseñada para medir el grado de aprendizaje de los estudiantes de los diferentes conceptos vistos en el espacio académico.
-Trabajo Nº 4 (Aplicación en contexto) Informe de investigación
-Materiales
-Diapositivas en PowerPoint de cada unidad temática y archivo en Word de la última unidad, en carpeta comprimida al inicio del espacio.
-Taller Nº 1, Taller Nº 2 y Taller Nº 3 archivos en Word.
-Taller Nº4 Informe de investigación construido por los estudiantes.
-Evaluación en plataforma.
-Bibliografía recomendada por el docente.
-Bibliografía recomendada por los estudiantes en cada foro semanal.
-Orientaciones
-Leer muy bien el microcurrículo.
-Leer las diapositivas de las unidades respectivas (Plataforma virtual)
-Revisar la bibliografía complementaria suministrada por el tutor
-Consultar e investigar en otras fuentes manuales y/o automatizadas sobre el contenido de    esta asignatura.
-Desarrollar las actividades propuestas en la guía
-Intercambiar inquietudes o aportes con sus compañeros y tutor (Foros, correo electrónico, chat de la plataforma)
-Participar activamente en los foros quincenales (En espacio de tiempo de sábado a sábado).
-Distribuir el tiempo para que puedan realizar las actividades de cada semana.
-Para presentar la evaluación tener sus apuntes a mano, una calculadora, lápiz y papel para solucionar los ejercicios, revisar la conectividad antes de presentarla.
-El informe de investigación se construirá en un foro paso a paso finalizando la Unidad Nº5
-</t>
-  </si>
-  <si>
-    <t>Las formas de evaluación deben ser de naturaleza múltiple.  Se citan algunas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuando algunas personas escuchan la palabra “estadística” inmediatamente piensan en promedio de notas, índice de accidentes, índice de mortalidad, tasas de nacimiento y otros indicadores comunes, en realidad esta rama de la estadística que utiliza números para describir hechos recibe el nombre de Estadística Descriptiva.
-La Estadística Descriptiva comprende primordialmente de la recolección, recopilación, ordenamiento, organización, tabulación, presentación, tratamiento matemático y análisis de datos con el objeto de describir las situaciones o hechos que han proporcionado la información recolectada, que a menudo es muy compleja.  Por lo general toman la forma de tablas, cuadros, gráficos, índices numéricos, tasas, proporciones, etc., que describen muy detalladamente lo que está sucediendo a una actividad comercial, biológica, industrial, de salud o de cualquier índole, referida siempre en una actividad de tiempo y espacio.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿De qué manera se puede utilizar la información para evaluar procesos y proponer alternativas de solución frente a situaciones irregulares?
-Recoger, tabular y organizar información para predecir situaciones y proponer alternativas de solución.
-A lo largo de este curso el estudiante estará en capacidad de: 
-Utilizar apropiadamente los diferentes términos estadísticos.
-Organizar e interpretar datos estadísticos en una tabla de distribución de frecuencias. 
-Determinar e interpretar medidas de tendencia central y de posición en una serie de datos estadísticos. 
-Elaborar gráficas de representación de la distribución de frecuencia de los datos Estadísticos.
-Calcular e interpretar las medidas de variabilidad en una serie de datos estadísticos.
-Construir la ecuación de regresión que representa el comportamiento de dos variables.
-Utilizar las etapas del proceso de investigación científica para proponer un informe de investigación.
-Seleccionar o elaborar un instrumento estadístico nos permita acepta o rechazar una hipótesis
-Elaborar un informe de investigación que reúna todos los conceptos estadísticos estudiados.
-Proponer alternativas de solución a problemas detectados.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conceptos generales y distribución de frecuencias para datos no agrupados en intervalos de clase
-Distribución de frecuencias para datos agrupados en intervalos de clase
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medidas de tendencia central y posición
-Medidas de dispersión y variabilidad
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gráficas estadísticas
-Regresión y Correlación
-Instrumentos estadísticos
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En este espacio académico los estudiantes deben elaborar trabajos de aplicación en contexto donde utilizarán las herramientas aprendidas a lo largo de la asignatura para evaluar y proponer soluciones a situaciones cotidianas.
-En actividades como: Trabajo Nº 3 de aplicación en contexto se aplican y evalúan las unidades 1, 2 y 3.
-Trabajo Nº 4 Informe de investigación el cual permite un acercamiento al proceso de investigación enfocado desde la estadística descriptiva y la investigación aplicada. (Se evalúan y aplican todas las unidades desarrolladas en el curso
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEJIA A. Dario. Estadística general aplicada a la educación. 
-MURRAY R. Spiegel. Probabilidades y Estadística. Serie Shaum.
-LINCOLN L. Chao. Estadística para las Ciencias Administrativas. Ed. Mc. Graw Hill      
-GARCIA P. ALVARO. Estadística. Universidad Industrial de Santander
-La propuesta en el foro respectivo por cada uno de los estudiantes.
-INSE. Métodos de investigación. Universidad de la Sabana.
-Hernández S. Roberto.  Fernández C. Carlos.  Baptista L. Pilar. Metodología de la investigación.  Mc Graw Hill.
-López G. Efraín.  El proceso de la investigación.  Universidad del Quindío
-Además de las anteriores, toda aquella propuesta por el estudiante en el foro respectivo a lo largo de la asignatura
-</t>
-  </si>
-  <si>
-    <t>1 semestre</t>
-  </si>
-  <si>
-    <t>2019-07-29- Mónica Valencia Parra – Julio César Castaño Marín. Actualización de la plantilla con el PAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lina María Castro Benavides
-Coordinadora de área
-</t>
-  </si>
-  <si>
-    <t>GESTIÓN DOCUMENTAL</t>
-  </si>
-  <si>
-    <t>Con el reconocimiento legal que los documentos institucionalizan las decisiones administrativas y los archivos constituyen una herramienta indispensable para la gestión administrativa, económica, política y cultural del Estado y la administración de justicia; son testimonio de los hechos y de las obras; documentan las personas, los derechos y las instituciones, se hace necesario que los futuros Profesionales en Ciencia de la Información y la Documentación, Archivística y Bibliotecología, adquieran los conocimientos y metodologías relacionados con la gestión de documentos de archivo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para el desarrollo de la asignatura Gestión Documental se entregarán: material de apoyo educativo, lecturas relacionadas con los temas trazados, desarrollo de talleres y trabajos en equipo donde el estudiante con base en el material facilitado y las investigaciones realizadas, enriquecerá los foros de participación, de tal manera que reconozca como un escenario de participación, discusión, extensión, y puesta en común de conceptos estudiados y mejores prácticas laborales con el fin de asimilar los conocimientos adquiridos en presente asignatura.
-Como parte integral del proceso de formación, el estudiante debe leer y analizar los artículos y material que la Docente dispondrá en la Plataforma y consultar otras fuentes de información como los portales recomendados en la bibliografía.
-El propósito, fortalecer el ser, hacer y el saber; que sean reconocidos en el ámbito laboral como Profesionales integrales.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con el fin de evidenciar los conocimientos adquiridos en el desarrollo de la asignatura, se llevarán a cabo diferentes evaluaciones con la presentación de las tareas en las fechas estipuladas.
-La tutora  por su parte, realizará la retroalimentación pertinente a medida que se desarrolle cada actividad, foro o actividad con el fin de ser tenida en cuenta por usted amig@ estudiante en el desarrollo de la Unidad que le siga a la misma. 
-Las Actividades  deben cumplir con los requisitos y fechas establecidas en cada actividad.
-Las tareas son individuales y algunas en parejas y como tal se deben  presentar. 
-No se reciben actividades fuera de plataforma, ni fuera de las fechas establecidas.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teniendo en cuenta que la gestión documental es un proceso transversal a toda organización, en la presente asignatura se estudiarán y analizarán los diferentes aspectos y componentes de la gestión de documentos incluyendo la normatividad que sobre esta materia rige en el país.
-Con la aprobación de la ley 594 de 2000 “Ley General de Archivos” los procesos de gestión documental se han ido articulando al interior de las organizaciones como herramientas de gestión, alineados con políticas, directrices y lineamientos que deben interactuarse con los sistemas integrados de gestión orientados a la mejora de los procesos organizacionales.
-Las normas NTC-ISO 30300 y 30301 establecen claramente en su introducción que: “La gestión documental, hace posible la eficiencia, la rendición de cuentas, la gestión de los riesgos y la continuidad del negocio. También permite a las organizaciones capitalizar el valor de sus recursos de información convirtiéndolos en activos comerciales y de conocimiento, y contribuyendo a la preservación de la memoria colectiva, en respuesta a los desafíos de entorno global y digital”. Partiendo de este concepto, el estudiante deberá desarrollar habilidades
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La identificación de riesgos inherentes a la Administración de la Gestión Documental, mediante el análisis del entorno, causas, efectos y su valoración frente a las probabilidades y consecuencias identificando los elementos relevantes para la valoración.
- La estructuración de indicadores de gestión
- La toma de decisiones relacionadas con las obligaciones que pudieren tener las empresas de acuerdo a su naturaleza jurídica. ¿Cómo conseguirlo? Mediante el conocimiento teórico práctico de los principios y fundamentos archivísticos aunado a los procesos de la gestión documental establecidos por el Archivo General de la Nación (AGN), como ente rector de la política archivista y obedeciendo a una estructura normalizada que permita la interacción con otros sistemas administrativos, de calidad y de gestión.
- Adquirir los conocimientos asociados a los procesos de Gestión Documental mediante el análisis de la legislación, los componentes administrativos, tecnológicos y de gestión con el fin de que presenten y gestionen estrategias al interior de las organizaciones relacionadas con el uso de la información confiable, oportuna y organizada garantizando así, el derecho de acceso a la información.
- Establecer el papel, la importancia y las interrelaciones que existen entre los procesos de Gestión Documental y la administración tanto a nivel técnico, de dirección, de calidad y de gestión.
- Identificar la normatividad archivística y conexa asociada a la Gestión Documental
- Adquirir elementos conceptuales y técnicos necesarios para el desarrollo de su gestión como Profesionales de la Información.
- Reconocer la Unidad de Correspondencia como parte integral de un PGD
- Determinar los criterios para la organización de los archivos de gestión en una entidad.
- Comprender las fases del ciclo vital de los documentos y la forma como se podrá acompañar y liderar un proceso de Gestión de Servicios Documentales.
- La asignatura Gestión Documental se relaciona con el propósito del Programa porque lleva al estudiante a reconocer en los procesos de gestión documental: planeación, producción, gestión y tramite, organización, transferencia, disposición de los documentos, preservación a largo plazo y valoración; la importancia de la administración de la información para la toma de decisiones.
- También se presenta una relación implícita relacionada con la identificación y valoración de los riesgos propios de la gestión de la información que el futuro Profesional deberá caracterizar al interior de los procesos de gestión documental con el fin de garantizar el derecho de acceso a la información.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La asignatura Gestión Documental se relaciona con el propósito del Programa porque lleva al estudiante a reconocer en los procesos de gestión documental: planeación, producción, gestión y tramite, organización, transferencia, disposición de los documentos, preservación a largo plazo y valoración; la importancia de la administración de la información para la toma de decisiones.
-También se presenta una relación implícita relacionada con la identificación y valoración de los riesgos propios de la gestión de la información que el futuro Profesional deberá caracterizar al interior de los procesos de gestión documental con el fin de garantizar el derecho de acceso a la información
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta asignatura se desarrollará a partir de 6 Unidades Temáticas:
-Unidad 1: Introducción a la Gestión Documental 
- Concepto sobre gestión Documental 
- Código de ética del Archivista
- Marco Normativo 
- Principios rectores de la Archivística 
- En la semana 1 se realizará la Bienvenida al espacio académico,  la socialización del Syllabus, y las actividades correspondientes a la Unidad 1.  
-Unidad 2: Componentes de un Programa de Gestión Documental 
- Principios del Proceso de Gestión Documental 
- Procesos de la Gestión Documental 
- Programa de Gestión Documental 
-Unidad 3: Implementación de los Programas de gestión Documental 
- Implementación de un PGD 
- Sistema de gestión Documental 
-Unidad 4: Comunicaciones Oficiales parte integral de la gestión Documental 
- Marco normativo  
- Unidad de correspondencia 
- Procedimientos 
-Unidad 5: Administración del Riesgo 
- Contexto de la administración de riesgos
- Esquema de la administración de riesgos
-Unidad 6: Gestión de Series Documentales 
- Clasificación de las series documentales 
- Historias laborales 
- Historias Clínicas Ocupacionales 
- Contratos
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ARCHIVO GENERAL DE LA NACION.  Ley 594 de 2000. Ley General de Archivos.
- ARCHIVO GENERAL DE LA NACIÓN. Manual de implementación de un Programa de Gestión Documental. —Bogotá: El Archivos, 2014.
- ARCHIVO GENERAL DE LA NACIÓN (Colombia). División de Clasificación y Descripción. Cartilla de clasificación documental. Editorial: Bogotá: Archivo General de la Nación, 2001. 28 p
- CABRERA DÉNIZ, M.D; RODRÍGUEZ ACEVEDO, J.M. y RUIZ DE GALARRETA TOVAR, P. La teoría desde la práctica. Nuevas reflexiones sobre el concepto de serie documental, Arch-e, 2011, Nº 5
- CRUZ MUNDET, José Ramón: “Manual de Archivística". Edición corregida y actualizada. Fundación Germán Sánchez Ruipérez. Madrid, 2001.  413 p.
- CRUZ MUNDET, J.R. La gestión de documentos en las organizaciones Madrid: Ediciones Pirámide, 2006
- HEREDIA HERRERA, Antonia: “Archivística General. Teoría y Práctica”. Diputación Provincial de Sevilla. 1995. Sevilla (España).
- VÁZQUEZ MURILLO, Manuel. Administración de Documentos de Archivos: Planteos para el siglo XXI/ 2ª ed. Corregida. Buenos Aires, 2006. 160 p
- TÉCNICAS Y CERTIFICACIÓN. Norma para la descripción de funciones. Editorial: ICONTEC: Archivo General de la Nación, 2014. 28 páginas. -------------- Norma para la descripción de funciones. Editorial: ICONTEC. Archivo General de la Nación, 2014. Gestión Document
-</t>
-  </si>
-  <si>
-    <t>ÁLVAREZ A., MARÍA JANETH. Hacia la funcionalidad del sistema de clasificación de archivos en los organismos de vigilancia y control de Colombia: una propuesta de investigación Disponible en: Códice: revista de la Facultad de Sistemas de Información y Documentación (Bogotá). -- Vol. 3, no. 1 (Ene./Jun. 2007). -- p. 63-71</t>
-  </si>
-  <si>
-    <t>Este syllabus tiene vigencia para el segundo período del 2017.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseño: Marlene Salazar Ramos 
-Evaluación: Dolly Rivera Chavez
-</t>
-  </si>
-  <si>
-    <t>SELECCIÓN DE TEXTOS: GÉNEROS Y
-EDADES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son muchas las situaciones que requieren un buen criterio del profesional CIDBA para seleccionar textos adecuados de acuerdo con la edad, género, intereses y necesidades del  público lector: preparar actividades de animación; orientar a los padres de familia acerca de los mejores libros y materiales para despertar en sus hijos el amor por la lectura; recomendar libros y guiar a los maestros acerca de los libros y materiales documentales que pueden apoyar su labor educativa; o seleccionar textos para dotar una colección, entre otras.
-Las Unidades de Información, espacios desde los cuales el profesional CIDBA desarrollará su labor de promotor, son espacios de intercambio e interacción sociocultural que, por su carácter, deben ser abiertos a las comunidades. Deben fortalecerse entonces como escenarios de formación de ciudadanos con capacidad de lectura, interesados por la cultura, el conocimiento y la autoformación. El líder de dichas Unidades de Información debe estar capacitado para elegir adecuadamente los libros con los que va a desarrollar su trabajo, elección que pasa por distinguir un texto literario de otros tipos de textos, reconocer la calidad de las ediciones (presentación, formato, ilustraciones) e identificar los libros adecuados para cada edad y cada gusto; considerando que los  intereses lectores resultan, en últimas, tan íntimos y personales como los lectores mismos.
-Otro aspecto fundamental para la selección de textos es aquel que tiene que ver con la reflexión acerca de la propia experiencia de lectura. En los análisis, encuentros, congresos, publicaciones, etc., realizados en torno a las diversas actividades de promoción y animación de lectura, se evidencia fuertemente la importancia de que el mediador sea una persona capacitada en su quehacer y apasionada por la lectura. Esta situación indica un reto mayor: los futuros profesionales CIDBA deben iniciar, si no lo recorren ya, el interesante pero difícil camino de asumir la lectura no como obligación o requerimiento sino como actividad propicia para el goce y el enriquecimiento cultural, puesto que no es posible considerar que un texto es de calidad solamente porque sus ilustraciones son llamativas o porque es más comercializado y más vendido que otros. Es necesario que el mediador entienda que la lectura permite una vivencia real, profunda y creativa de la experiencia humana y por ello no todos los textos existentes en el mercado son de calidad
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De acuerdo a los Lineamientos de la Estrategia Virtual de la Universidad del Quindío,  la formación en Ambientes Virtuales de Aprendizaje está centrada en el aprendizaje y orientada bajo una concepción pedagógica construccionista. 
-Esta concepción pedagógica se basa en el Constructivismo (se construyen conocimientos al interactuar con el entorno y se refuerzan estos conocimientos al usarlos) y en el Construccionismo (el aprendizaje es particularmente efectivo cuando se adquiere construyendo algo que debe llegar a otros).  
-Para alcanzar estos conocimientos, se potencian saberes y competencias a través de Metodologías Activas (Aprendizaje Basado en Tareas de Trabajo Independiente ABTTI y Aprendizaje Basado en Tareas de Trabajo Cooperativo ABTTC – Aprendizaje Basado en Problemas, Método del Caso y Aprendizaje por Proyectos Colaborativos -) que promueve el Aprendizaje Significativo, Autónomo y Colaborativo.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las actividades y sus respectivos criterios de evaluación para este espacio académico son los siguientes:
-Foros (evaluativo y de estudio)
- Capacidad del estudiante para comprender, analizar, reflexionar, criticar y proponer frente a los diversos contenidos
- Capacidad del estudiante para investigar y presentar fuentes de información
- Normas básicas de presentación, redacción, ortografía
- Cumplimiento de la Norma APA para citar y referenciar
- Cumplimiento de las normas del Foro 
-Taller escrito
- Capacidad del estudiante para comprender, analizar, reflexionar, criticar y proponer frente a los diversos contenidos
- Apropiación de conocimientos
- Normas básicas de presentación, redacción y ortografía
- Cumplimiento de la Norma APA para citar y referenciar
-Evaluación en línea (Tipo Saber pro)
- Capacidad del estudiante para comprender, analizar, reflexionar, criticar y proponer frente a los diversos contenidos
- Apropiación de conocimientos
-Fichas de lectura (Trabajo grupal)
- Construcción de las fichas de lectura
- Calidad de los textos seleccionados
- Normas básicas de presentación, redacción y ortografía
-Video
- Capacidad del estudiante para evidenciar sus aprendizajes
- Calidad del texto presentado
- Creatividad de la actividad de animación
-</t>
-  </si>
-  <si>
-    <t>Selección de textos: géneros y edades es un espacio académico de carácter teórico-práctico en el cual los futuros profesionales en Ciencia de la Información y la Documentación, Bibliotecología y Archivística encontrarán herramientas y desarrollarán competencias que les permitirán desempeñarse efectivamente en su labor como promotores de lectura, especialmente en lo referente al manejo de diferentes tipos de textos y públicos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Al finalizar el proceso formativo el estudiante: 
- Adquiere, ejecuta y construye criterios de selección y evaluación de diversos tipos de textos de acuerdo con las características de sus potenciales lectores.
- Identifica las particularidades de los distintos tipos de textos y géneros literarios. 
- Selecciona textos de calidad para sus actividades de promoción y animación a la lectura.
- Fortalece su ejercicio como promotor y animador de lectura.
- Comprende las ventajas de la lectura literaria como experiencia estética y como ejercicio de fortalecimiento intelectual
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Géneros literarios
- Tipologías textuales
- Lectura como experiencia estética
- Lectura eferente
- Criterios de evaluación y selección de textos
- Literatura infantil y juvenil
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Selección de textos para actividades de animación a la lectura
- Elaboración de fichas de lectura
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Experiencia personal de lectura 
- El profesional CIDBA como mediador entre los libros y los lectores
-</t>
-  </si>
-  <si>
-    <t>El proceso de selección de textos, géneros y edades  nos permite hacer un proceso de interpretación del entorno y construir el sentido que a él le damos, en este espacio académico busca que al finalizar el proceso cada estudiante haga un ejercicio de aplicación proyectado a su quehacer profesional donde aplique los parámetros teóricos y los identifique y sustente en un contexto real. Mediante la realización de las distintas actividades teórico-prácticas se fomenta la investigación, el autoaprendizaje y la autorregulación del estudiante y el trabajo colaborativo como parte fundamental del aprendizaje virtual y la plataforma MOODLE.</t>
-  </si>
-  <si>
-    <t>esta en el cronograma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arguelles, J. (2006) Ustedes que leen. Controversias y mandatos sobre el libro y la lectura. México: Océano. 244 p.
-Campo, M. F. (2013) Leer para comprender, escribir para transformar. Palabras que abren nuevos caminos en la escuela. Bogotá: Ministerio de Educación Nacional. 
-Carranza, M. (2007). Algunas ideas sobre la selección de textos literarios. En Imaginaria. Recuperado de: http://www.imaginaria.com.ar/20/2/seleccion-de-textos-literarios.htm 
-Cervantes, G. (2005) La importancia del vínculo emocional. En: Memorias 3° Encuentro Internacional Sobre Bibliotecas.  La lectura en niños y jóvenes y el papel de la biblioteca pública  Ciudad de México: Consejo Nacional Para La Cultura Y Las Artes.
-Domingo, J. (2006) Memoria del Tercer Encuentro Internacional sobre Bibliotecas Públicas: La lectura en niños y jóvenes y el papel de la biblioteca. México: Consejo Nacional para la Cultura y las Artes, Dirección General de Bibliotecas.
-Fundación Alonso Quijano. La lectura por edades. Recuperado de: http://www.alonsoquijano.org/cursos2004/animateca_v2/ponencias/TRABAJOS%20FINAL/ESCENARIO%202/PARTE%20V/TEMA%2013/1%20LA%20LECTURA%20POR%20EDADES/lectura%20por%20edades.pdf 
-Lopera, G. (1999).  Selección de libros infantiles y juveniles. Comfenalco. Antioquia.
-Lluch, .G; Chaparro, J; Rincón, M. C; Rodríguez, C; Victorino, A (2009) Cómo reconocer los buenos libros para niños y jóvenes. Orientaciones de una investigación de Fundalectura. Bogotá: Fundalectura.
-Lluch, G. (2010.) 10 Consejos para seleccionar las lecturas. Secundaria. Docentes. Madrid: Ministerio de Educación, Leer.es. Recuperado de: http://leer.es/documents/235507/247059/art_prof_eso_10consejos_gemmalluch.pdf/52dc75c9-6230-4fd1-8096-3916050f33a1  
-Lluch, G. (2010). 10 Consejos para seleccionar las lecturas. Familias. Madrid: Ministerio de Educación, Leer.es. Recuperado de: http://familias.leer.es/files/2010/07/art_fam_10consejosparaseleccionarlaslecturas_gemmalluch.pdf
-MEN (2012). Criterios para seleccionar materiales de lectura y conformar colecciones para la primera infancia 2012
-MEN (2013). Leer para comprender, escribir para transformar: palabras que abren nuevos caminos en la escuela. 1ª ed.  Bogotá. Ministerio de Educación Nacional.
-Ospina, W. (s.f.). Lo que entregan los libros. Libro al viento. Recuperado de: http://repositoriosed.educacionbogota.edu.co/jspui/bitstream/123456789/86/1/leeryescribir.pdf 
-Pennac, D. (1996)  Como una novela. Bogotá: Norma, 1996.
-Petit, M; Docampo, X. (2002)  Pero y Qué Buscan Nuestros Niños En Sus Libros? México: CONACULTA, Dirección General de Publicaciones.
-Robledo, B. (2008) Evaluación y selección de libros para la promoción y animación a la lectura. En: II Encuentro de promotores de Lectura. Medellín: Fondo Editorial Comfenalco Antioquia.
-Rodríguez, G. (2007) La biblioteca pública: análisis a manifiestos y directrices. Medellín: Fondo Editorial Comfenalco Antioquia.
-Rodríguez, G. (2011) Bibliotecas vivas: la biblioteca pública que queremos. Bogotá: Ministerio de Cultura, Biblioteca Nacional de Colombia.   Recuperado de: http://www.bibliotecanacional.gov.co/caja-herramientas/sites/default/files/recursos/La%20biblioteca%20publica%20que%20queremos.pdf
-Sainz, L (2005) La importancia del mediador: una experiencia en la formación de lectores En: Revista de Educación, núm. extraordinario 2005, pp. 357-362
-Stapich, E ; Cañon, M. (2011) Infancia, lectura y mercado. En: Revista Pilquen • Sección Ciencias Sociales • Año XIII • Nº 14, 2011
-Trelease, J. (s.f.) Manual de la lectura en voz alta. Bogotá: Fundalectura. 423 p.
-Yepes, B. (1995) Propuesta para un taller sobre materiales de lectura para niños y jóvenes. Medellín: Fondo Editorial Comfenalco Antioquia
-</t>
-  </si>
-  <si>
-    <t>Julio 28 de 2017 -  Actualización de la plantilla acorde con la PAC- Lic. Mónica Murillo Sandoval - Docente</t>
-  </si>
-  <si>
-    <t>TEORÍA DE SISTEMAS</t>
-  </si>
-  <si>
-    <t>En la actualidad, todas las organizaciones desarrollan o adquieren sistemas de información que apoyen y fortalezcan su negocio, prácticamente se soportan en ellos. Es por esto que se convierte en un reto para las organizaciones implementar SI que cumplan con los requisitos de la organización, lo que significa inversión de tiempo, esfuerzo y dinero antes de invertir en un SI. En razón a que se deben tener en cuenta los SI existentes dentro de la organización y deben ser integrados entre sí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspectos generales que se tienen en cuenta para el desarrollo del curso. En la medida que se van trabajando los diferentes ejes temáticos de la asignatura también se irán desarrollando diferentes actividades como complemento al conocimiento adquirido, entre estas actividades encontrarán Foros de participación activa, talleres, evaluaciones, trabajos y consultas.  
-Por ser un programa de educación virtual, se hace valiosa la implementación de actividades tipo taller; ellos estarán disponibles en la plataforma en la medida en que se va estudiando cada uno de los tópicos propuestos para la asignatura.   
-La efectividad de los mismos depende de una actitud crítica y propositiva como lector de los nuevos sistemas de información y comunicación de la actual cultura.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El rol que cumple un profesional en ciencia de la información dentro de una organización es vital, en razón a que hace parte del equipo responsable de identificar, entender y especificar los requerimientos de información del negocio, los requisitos funcionales del sistema de información, y de participar en el modelamiento de datos y de información. Y es que tradicionalmente, en una organización se concibe al dinero y a las personas como activos reales que aportan valor, sin embargo, este paradigma ha cambiado, y los datos y la información se han unido a este gran conjunto, y actualmente son reconocidos por el alto valor que imprimen para alcanzar sus objetivos.
-La diferencia entre tomar decisiones basados en información bien concebida, y planeada, o tomar decisiones sin la información suficiente o de baja calidad, se verá reflejada en la efectividad de la decisión. Por lo tanto, la ausencia de información representa pérdidas con profundos impactos potenciales sobre la rentabilidad y efectividad operacional de cualquier organización.
-Hoy en día las organizaciones toman sus decisiones basadas en información de calidad, esto hace que se creen ventajas competitivas gracias a un mejor conocimiento de sus clientes, usos innovadores de la información, y eficiencias a nivel operacional. Los negocios usan los datos para conocer mejor los productos y servicios, y controlar sus riesgos. 
-Los gobiernos, las instituciones educativas, las organizaciones sin ánimo de lucro también necesitan alta calidad de la información para guiar sus actividades operacionales, técnicas y estratégicas. Si las organizaciones necesitan e incrementan su dependencia en los datos, se requiere establecer claramente el valor y uso de la información a su interior, por lo tanto se requiere conocer acerca de la concepción, análisis, diseño e implementación de un sistema de información que satisfaga sus requisitos
-En la actualidad, todas las organizaciones desarrollan o adquieren sistemas de información que apoyen y fortalezcan su negocio, prácticamente se soportan en ellos. Es por esto que se convierte en un reto para las organizaciones implementar SI que cumplan con los requisitos de la organización, lo que significa inversión de tiempo, esfuerzo y dinero antes de invertir en un SI. En razón a que se deben tener en cuenta los SI existentes dentro de la organización y deben ser integrados entre sí
-</t>
-  </si>
-  <si>
-    <t>¿Se puede lograr el conocimiento de la Sistemas y sus principales conceptos y su aplicabilidad dentro del entorno práctico de la Administración de Información, la Bibliotecología y la Archivística?</t>
-  </si>
-  <si>
-    <t>El Programa de Ciencia de la Información y la Documentación, Bibliotecología y Archivística  aborda las dimensiones de Extensión e Investigación a través de Proyectos de Extensión y de Investigación. Igualmente, el semillero de investigación donde los estudiantes tienen la oportunidad de presentar sus propuestas y ejecutar los proyectos.</t>
-  </si>
-  <si>
-    <t>Unidad 1. Generalidades de los sistemas de información       Unidad 2. Componentes de los sistemas de información    Unidad 3. Bloques de un sistema de información    Unidad 4. Ciclo de vida de un sistema de información</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kendall &amp; Kendall. Análisis y Diseño de Sistemas, Octava Edición. Prentice Hall. 2011
-James A. Senn. Análisis y Diseño de Sistemas de Información, Segunda Edición Mc. Graw-Hill
-http://www.econlink.com.ar/sistemas-informacion/definicion  - 
-http://www.vharj.freeservers.com/sistemas.htm - 
-Competencias y aptitudes de los profesionales de información y documentación. Euro-referencial en información y documentación. Segunda edición revisada. 2004
-Whitten Bentley. System Analysis and Design Methods 7th. MacGraw Hill. 2007
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio de clases 1 de agosto de 2017 al 24 de noviembre de 2017 </t>
-  </si>
-  <si>
-    <t>Julio de 2017 - Alejandra Giraldo Gaviria – Actualización de la plantilla ajustada al PAC</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN BIBLIOGRÁFICA
-NORMALIZADA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Descripción Bibliográfica Normalizada es indispensable para el  control de todos los recursos publicados en múltiple formatos y soportes de información,  con el fin de que  el universo bibliográfico se encuentre disponible y sea accesible de manera ágil y oportuna. 
-Una buena descripción bibliográfica permite la recuperación, acceso y divulgación de las fuentes de información por parte de los diversos usuarios y sirve de puente para realizar intercambio de la información bibliográfica entre las Unidades de Información                                                              Para el futuro profesional en CIDBA es indispensable el dominio de los recursos que aporta la asignatura Descripción Bibliográfica Normalizada. A partir de sus contenidos el estudiante adquiere las siguientes competencias:
-Manejo de  reglas y normas internacionales coherentes para la descripción de los diversos tipos de recursos publicados. 
-Uniformidad en la medida de lo posible y especificaciones concretas para determinados tipos de recursos bibliográficos, según lo requiera su descripción. 
-Capacidad para abordar, comprender y aplicar los conceptos clave así  como los diferentes instrumentos utilizados para realizar una buena descripción documental, que contribuya de manera eficaz a la satisfacción de las necesidades de información de los usuarios.  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La metodología de aprendizaje en Descripción Bibliográfica Normalizada se basa en el estudio y la aplicación de procedimientos para el análisis y catalogación de los documentos que forman parte de un acervo documental, que se visualizan en forma física en las bibliotecas y en forma digital a través del Catálogo de acceso público en línea (OPAC). Para ello se tendrán en cuenta las tipologías, problemáticas y la normativa de desarrollo, análisis y catalogación que internacionalmente respalda la Descripción Bibliográfica Normalizada.
-El proceso comprende las siguientes pautas:
-Formación de conceptos. 
-Elaboración de procedimientos de ingreso de material, depuración de bases de datos, registro en las plantillas correspondientes 
-Resolución de problemas.
-Las dos primeras, como formas predominantes en la adquisición de conocimiento y habilidades (Saber) y la tercera, junto con la ejercitación en general, como la forma predominante en la fijación de dichos conocimientos y habilidades (Saber hacer). 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">García, Ageo. (2002). Formato MARC 21 para el registro de autoridades. Sitio  
-Web visitado 14 de junio 2016, de http://cictd.uaslp.mx/autoridades/MARCslp.pdf
-Gil Leiva, I. (2008). Manual de Indización. Teoría y práctica. España. Trea.  
-Martínez García, M &amp; Olaran Múgica, M. (2007). Manual de catalogación en formato MARC : IBERMARC y MARC 21: monografías impresas modernas. 2ª ed.  Madrid : Arco-Libros  
-Méndez Rodríguez, E. M. [2002]. Metadatos y recuperación de información: Estándares, problemas y aplicabilidad en bibliotecas digitales.
-Ríos Hilario, A.B. (2006). Prácticas de catalogación: supuestos monográficos  de acuerdo con las ediciones vigentes de las reglas de catalogación y el  formato IBERMARC. España. Trea.    
-Reglas de catalogación angloamericanas. ( 2004) Bogotá. Rojas Eberhard
-Spedalieri, G. (2007). Catalogación de monografías impresas. 1. ed. Buenos Aires. Alfagrama http://es.slideshare.net/LucaLubna/t5-25306592  .  Consultado 16 de junio de 2016
-https://www.oclc.org/es-americalatina/rda/about.html. Consultado 16 de junio de 2016
-http://www.sicht.ucv.ve:8080/OPAC/listado/index.php?cod1=V&amp;cod2=H.  Consultado junio 16 de 2016.  En este enlace encontrará ,las herramientas de uso para la descripción bibliográfica normalizada, que le permitirá ampliar sobre el tema del curso, tales como: Formato Marc 21 Conciso para Datos Bibliográficos Biblioteca del Congreso, Descripción Bibliográfica Internacional Normalizada (ISBD)
- Federación Internacional de Asociaciones de Bibliotecarios e Instituciones (IFLA), entre otros.
-</t>
-  </si>
-  <si>
-    <t>LENGUAJES, ANÁLISIS Y RECUPERACIÓN
-DE LA INFORMACIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El conocimiento y aplicación de LARI permite el manejo adecuado de los documentos en una biblioteca y de sus bases de datos; por medio de ellos se conoce qué existe dentro de una unidad de información sobre determinado tema. 
-El análisis documental es un proceso mediante el cual se representan los puntos de acceso que tienen los documentos, mediante el uso de símbolos o términos, con el fin de recuperarlos y ponerlos a disposición del usuario.
-El análisis es el requisito previo para poner a disposición de quien lo necesita, la información que se genera. Para el estudiante de CIDBA, consiste en desglosar los documentos en sus partes, indicando sus aspectos más relevantes y cuáles resultan de considerable valor al momento de su posterior recuperación. Sus componentes, usuario-información, precisan de una información compatible con la terminología que utilizan para expresar el contenido por medio del lenguaje normalizado; de ahí la importancia de los LARI en esta carrera
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En el desarrollo de este espacio académico  se tendrán en cuenta interactividades e interacciones que integren el conocimiento y la transferencia de información.
-El trabajo individual será un factor fundamental para el manejo de habilidades y competencias; las actividades propuestas en la plataforma permitirán adquirir y afianzar los temas en cada unidad. Las mismas estarán disponibles en la medida en que se avanza en cada uno de los ejes temáticos propuestos. Por todo lo anterior, el aprendizaje efectivo de los temas propuestos depende de su actitud crítica y propositiva como lector de los nuevos sistemas de información y comunicación de nuestra cultura.
-Los ejercicios evaluativos deberán ser presentados en algunas ocasiones de manera individual y en otras implicarán un trabajo conjunto. Para la presentación de los trabajos es imprescindible aplicar una adecuada redacción, puntuación y ortografía
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por cada una de las actividades evaluativas se referirán las indicaciones pertinentes para que los estudiantes puedan cumplir con los objetivos trazados.
-Igualmente, cada unidad contará con un foro de ayuda en el cual se resolverán las inquietudes que surjan en el desarrollo de la asignatura
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es necesario realizar un buen análisis y recuperación de la información, ya que la producción documental ha aumentado en los últimos años, por lo que se han generado otras necesidades, sistemas y técnicas de tratamiento documentales. Por tanto, este proceso debe estar fundamentado en unos elementos teóricos y prácticos, con el propósito de que los estudiantes de Ciencia de la información desarrollen las competencias necesarias para aplicar en el contexto de su quehacer profesional, los saberes y herramientas que le permitirán realizar una correcta clasificación de los contenidos. 
-LARI (Lenguajes, Análisis y Recuperación de la Información) se enfoca en los lenguajes controlados artificiales, cuya función es describir o expresar los temas o materias centrales de los documentos y sus características formales; en otros términos, ilustra el proceso mediante el cual la información es seleccionada y organizada para que pueda ser localizada fácilmente, de manera posterior, tanto por el bibliotecólogo como por el usuario final
-</t>
-  </si>
-  <si>
-    <t>El programa CIDBA busca formar profesionales competentes desde una perspectiva teórico-práctica, para manejar el ciclo de la información en cada una de sus diferentes etapas: entrada, proceso y salida. Se brindan los elementos conceptuales para el manejo y organización de la información; condición necesaria para el cumplimiento de las mencionadas etapas. Mediante la realización de las distintas actividades teórico-prácticas se fomenta la investigación, el autoaprendizaje y la autorregulación del estudiante y el trabajo colaborativo como parte fundamental del aprendizaje virtual y la plataforma MOODLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Competencias conceptuales
-• Identifica  los mecanismos básicos de los procesos de indización
-• Determina criterios sobre conceptos y términos. 
-• Analiza y recupera información a partir de los LARI.
-• El estudiante  adquiere  las herramientas necesarias para la construcción de los Lenguajes, análisis y recuperación de la información LARI, con sus distintos términos y particularidades
-• Conoce qué son los lenguajes documentales, sus funciones y sus componentes.
-• Reconoce e identifica  los tesauros.
-• Identifica y aplica el uso Descriptores dentro de los procesos de indización
-Competencias procedimentales
-• Utiliza los  mecanismos básicos de los procesos de indización.
-• Aplica los lenguajes documentales, sus funciones  y sus componentes para organizar la información y ponerla a disposición del usuario
-• Aplica  los lenguajes documentales, el análisis y recuperación de información (LARI)  de manera adecuada y significativa.
-• Compara distintas formas de representar una unidad de información y evalúa la más conveniente.
-• Maneja  el ciclo de la información en cada una de sus diferentes etapas: entrada, proceso y salida
-• El estudiante identifica  los conceptos del tesauro, elementos, tipología y sus relaciones para aplicarlo en casos concretos y reales
-Competencias actitudinales
-• Capacidad de análisis de su realidad
-• Sentido de responsabilidad 
-• Capacidad de trabajo en equipos interdisciplinares
-• El estudiante presenta sus trabajos, participa en los foros de manera activa, responsable y ética
-</t>
-  </si>
-  <si>
-    <t>Adquirir  las suficientes capacidades y conocimientos en LARI (Lenguajes, Análisis y Recuperación de la Información) para organizar la información y ponerla a disposición del usuario.</t>
-  </si>
-  <si>
-    <t>Desarrollar los suficientes elementos para aplicar en el contexto real LARI (Lenguajes, Análisis y Recuperación de la Información) en un contexto laboral.</t>
-  </si>
-  <si>
-    <t>Apropiarse de  los elementos y conocimientos necesarios para una educación integral y permitan la formación holística de los estudiantes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amat- Noguera, Nuria. (s.f.) Teoría de la documentación y fundamentos de la Ciencia de la información. Barcelona.
-Blázquez Ochando, Manuel. (2013). [Monografía] Técnicas avanzadas de recuperación de información: procesos, técnicas y métodos / Manuel Blázquez Ochando. – Madrid: mblazquez.es. Universidad Complutense de Madrid. Facultad de Ciencias de la Documentación.
-Espinosa Ricardo, L. (1989) Lenguajes de Análisis y Recuperación de información. Armenia: Universidad del Quindío.
-Godoy Velasco, M. (s.f.) La indización en la documentación. Universidad Carlos III. Consultado el 24 de enero de 2017 en http://www.galeon.com/indizacion/indizacion.html,
-Maniez, J. (1992). Lenguajes documentales y de clasificación: Concepción, construcción, y utilización en los sistemas documentales. Madrid: Fundación Germán Sánchez Ruipérez.
-        García Gutiérrez, A. (1984). Lingüística documental: aplicación a la documentación de la comunicación social.
-Repositorio Institucional Universidad de Alicante. (s.f). Tema 2: El proceso documental: del análisis a la recuperación de la información. Recuperado el 24 de enero de 2017 de https://rua.ua.es/dspace/bitstream/10045/15241/6/UNIDAD-2-Documentaci%C3%B3n-Informativa.pdf
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Julio 28 de 2017-Actualización de la plantilla acorde con la PAC- Esp. Alejandra María Parra Sánchez-Docente
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esp. Patricia Villegas Celis- Coordinadora de Área Acto Lector
-</t>
-  </si>
-  <si>
-    <t>PUBLICACIONES PERIÓDICAS</t>
-  </si>
-  <si>
-    <t>CLUBES Y RINCONES DE LECTURA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para el programa de Ciencia de la Información y la Documentación, Bibliotecología y Archivística, la formación de sus estudiantes implica dotar a los futuros profesionales de las habilidades que les permitirán desenvolverse adecuadamente en un mercado bastante competido y dinámico. En dicho escenario la habilidad para leer y escribir se plantea como construcción de sentido e instrumento reflexivo para contribuir desde nuestra profesión a  aportar escenarios de equidad que beneficien a las comunidades de usuarios de las diversas unidades de información donde nos desempeñamos.
-Las personas  habituadas a leer, manifiestan un alto grado de concentración, gozan de un repertorio verbal muy amplio y están dotadas de mejores condiciones para comunicarse con los demás de manera oral o escrita.  Por otra parte, la lectura abre las puertas al conocimiento, desarrolla la imaginación y la creatividad, fortalece la capacidad de comprensión y nos hace mejores ciudadanos. 
-El espacio académico de “Clubes y Rincones de Lectura”  incentiva a los estudiantes para que hagan contacto con estrategias encaminadas a instaurar programas de promoción lectora en sus ámbitos de influencia. El propósito es contribuir a que niños y adultos, a través del trabajo de las unidades de información, tengan acceso a prácticas de lectura donde los participantes actúen como sujetos activos de un proceso que les permita descubrir sus potencialidades como lectores y el valor que la lectura de textos escritos, especialmente litera tura, tiene para sus vidas. 
-El espacio académico de “Clubes y Rincones de Lectura”  contribuye, desde la reflexión  y la práctica, a la formación de profesionales íntegros que interactúen con sus realidades locales para propiciar el fortalecimiento del acto lector en públicos diversos. Todo ello en consonancia con el lineamiento teleológico de procurar académicamente el bienestar de la sociedad a la que sirven las unidades de información y los profesionales que egresan del programa Ciencia de la Información y la documentación.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desde el paradigma del e-learning y el código ético de la profesión, el espacio académico Clubes y Rincones de Lectura desarrolla su propuesta considerando un diseño formativo que provee recursos electrónicos seleccionados por la calidad y pertinencia de sus contenidos y una serie de actividades graduadas que: incentivan el pensamiento crítico; estimulan la consulta de los entornos locales donde habitan los estudiantes y promueven el trabajo colaborativo.
-Las actividades comprenden: 
-• Foro de formación de grupos; 
-• Foros académicos para revisión de conocimientos previos
-• Lectura individual de textos; 
-• Producción grupal escrita; 
-• Foros académicos de sustentación
-• Informes académicos, 
-• Revisión de videos y blogs, 
-• Retroalimentaciones
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El desarrollo de la asignatura combina la interactividad de la metodología virtual y los recursos electrónicos más pertinentes, para que los estudiantes hagan comprensión de los contenidos básicos y apropiación de experiencias formativas. Para lograrlo se utilizarán los recursos de la plataforma MOODLE, los materiales de apoyo y el acompañamiento tutorial.  El espacio académico comprende tres unidades que abordan de manera básica los componentes de una estrategia de promoción lectora denominada Clubes y rincones de lectura que tiene reconocimiento internacional. 
-Se propiciarán espacios para la reflexión sobre los conceptos de lectura y la gestión de un club de Lectores.  El sentido de trabajar en grupo corresponde a la intención de estimular la interacción entre los estudiantes para que se escuchen entre compañeros, intercambien información, analicen y valoren otros puntos de vista porque los talentos distintos amplían la visión. La idea es que se organicen para realizar las actividades y cooperen con otros estudiantes. La propuesta metodológica se soporta en estrategias de construcción grupal. La actividad tutorial es de facilitación frente a la consulta,   complementación y retroalimentación de los contenidos propuestos en el espacio académico.
-Los porcentajes estipulados son obligatorios. El número de evaluaciones, foros e informes para llegar a los porcentajes estipulados se concertará con los estudiantes
-</t>
-  </si>
-  <si>
-    <t>En el proceso de formación de los profesionales en Ciencia de la Información y la Documentación de la Universidad del Quindío, el componente de Acto Lector constituye una iniciativa diferencial y un valor agregado de su propuesta académica. El propósito de “Clubes y Rincones de Lectura”  es brindar elementos de juicio para contribuir a  la activación de espacios de socialización de la lectura como experiencia significativa de crecimiento articulado no sólo en el espacio académico sino y sobre todo en el ámbito social en el cual los profesionales se desempeñarán</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desde la perspectiva del saber y el saber hacer se trata de ofrecer a los estudiantes de Ciencia de la Información y la Documentación, Bibliotecología y Archivística las herramientas necesarias para que respecto al acto lector incentiven:
-• La generación de espacios para relacionarse con otros de manera cada vez más comprensiva y justa;
-• La capacidad de resolver problemas cotidianos.
-• La contribución  a que diversos ciudadanos encuentren en la lectura un mundo que les permita  actuar  constructivamente al interior de una sociedad más democrática 
-• La inclusión y el respeto por las  diferencias en el entorno cercano y en  su comunidad.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primera Unidad
-• Identificar los conceptos de Lectura como acto complejo y Lectura crítica.
-• Diferenciar Promoción de la lectura y Animación a la lectura.
-• Reflexionar sobre las responsabilidades profesionales del bibliotecólogo y su rol social en las unidades de información
-Segunda Unidad
-• Conceptualizar el Club de Lectores y las reglas de juego que lo sustentan
-• Explorar las realidades locales sobre promoción, animación y clubes de lectura.
-Tercera Unidad
-• Identificar variables socioeconómicas locales y establecer un grupo objetivo con necesidades de lectura puntuales.
-• Diseñar un Club de Lectura para el entorno local de los estudiantes del Programa. 
-• Efectuar selección de textos para la programación lectora del Club diseñado.
-• Desarrollar una estrategia pertinente de divulgación para la promoción de proyectos lectores
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALONSO, Samuel: “Club de lectores y El mono gráfico, dos propuestas de escritura en el CILIJ”. 6ª Jornadas de Bibliotecas Infantiles y Escolares. Salamanca : Fundación Germán Sánchez Ruipérez, 1999, pp. 105-110
-ARELLANO YANGUAS, Villar: “El Club de Lectores: un instrumento para socializar la lectura”,  en  Educación y Biblioteca, n. 61 (oct. 1995), pp. 57-58
-CALVO ALONSO-CORTÉS, Blanca: “Excepciones que transforman las reglas: los clubs de lectura”, en  Educación y Biblioteca, n. 35 (marzo 1993), pp. 63-65
-CALVO ALONSO-CORTÉS, Blanca. “Receta para un club de lectura”. En: http://travesia.mcu.es/receta.asp (05/12/2002)
-CANDAMIO GONZÁLEZ, Antonieta: “Los clubes de lectura”, en Educación y Biblioteca. Madrid, n. 208 (2003), pp. 50-51
-Los clubes de lectura, alma de las actividades de las bibliotecas. En: Anaquel, n. 18, (jun.-oct. 2002), pp. 3-10
-En marcha el Club Universitario de Lectura. En: Leer x Leer, n. 10 (abr. 2002),  p. 2.
-Libros altamente recomendados 2017 (FUNDALECTURA) [en línea], 04/05/2017 [revisado 29 de julio 2017]. Disponible en Internet: http://revistababar.com/wp/libros-altamente-recomendados-2017-fundalectura 
-MERINO MERINO, P. y ALONSO POLANCO, José Luis: El placer de la lectura. Santander: Librería Estudio, 1992. Primer Encuentro de Clubes de Lectura: Biblioteca Pública del Estado de Guadalajara- En: Educación y Biblioteca, n. 113 (2000), pp. 4-12
-RODRÍGUEZ RIVERO, M. Leer para discutir, discutir para leer En: El País. Suplemento Babelia, (31 de julio de 1999),  p. 3.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esp. Martha Lucía Usaquén Ramos - Docente.
-Esp. Patricia Villegas Celis- Coordinadora de Área Acto Lector
-</t>
-  </si>
 </sst>
 </file>
 
@@ -1828,30 +1224,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1866,7 +1244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1881,17 +1259,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2172,48 +1540,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ17"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="50.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2323,8 +1691,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>141210101</v>
       </c>
       <c r="B2" t="s">
@@ -2427,7 +1795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>141210102</v>
       </c>
@@ -2531,7 +1899,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>14121015</v>
       </c>
@@ -2635,7 +2003,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>141220104</v>
       </c>
@@ -2739,7 +2107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>141210204</v>
       </c>
@@ -2842,8 +2210,11 @@
       <c r="AH6" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="AI6" s="6">
+        <v>141210101</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>141210205</v>
       </c>
@@ -2943,11 +2314,11 @@
       <c r="AH7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AI7">
-        <v>1</v>
+      <c r="AJ7" s="6">
+        <v>141210101</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>141210206</v>
       </c>
@@ -3032,9 +2403,6 @@
       <c r="AB8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AC8" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="AD8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3051,7 +2419,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>141210301</v>
       </c>
@@ -3064,737 +2432,11 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9">
-        <v>3</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9" s="6"/>
-      <c r="T9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="W9" s="1" t="s">
         <v>120</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>141210303</v>
-      </c>
-      <c r="B10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF10" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>141210304</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6"/>
-      <c r="T11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="AF11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH11" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>141210305</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC12" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG12" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>141210306</v>
-      </c>
-      <c r="B13" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13" s="6"/>
-      <c r="T13" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG13" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>141220302</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AD14" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>141220404</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15" s="6"/>
-      <c r="T15" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD15" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG15" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH15" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
-        <v>141220405</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>141210503</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17" s="6"/>
-      <c r="T17" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="X17" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC17" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH17" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AI17">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>